<commit_message>
sizing cost matrix started
</commit_message>
<xml_diff>
--- a/data/fuel-mixing-experiments.xlsx
+++ b/data/fuel-mixing-experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos\upstream-salmon-rocket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBA2865-618E-4715-8AF9-9237D6DD5F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B76C1A-D66E-45E9-A80E-FE98056295B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="5910" windowWidth="32550" windowHeight="17640" xr2:uid="{8094CE1F-7225-44C2-8392-BEB4E291545F}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="17355" xr2:uid="{8094CE1F-7225-44C2-8392-BEB4E291545F}"/>
   </bookViews>
   <sheets>
     <sheet name="Salmon Isopropyl Mixing Test 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Salmon Mass</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Density</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242EF89F-5CE8-4268-BB84-4BF91496249E}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +454,7 @@
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -482,8 +485,11 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -512,7 +518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -533,8 +539,12 @@
       <c r="I3">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f>I3/H3</f>
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>61.7</v>
       </c>
@@ -548,38 +558,42 @@
       <c r="I4">
         <v>27.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f>I4/H4</f>
+        <v>0.92666666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" t="e">
         <f>B10/(B10+C10)</f>
         <v>#DIV/0!</v>

</xml_diff>